<commit_message>
meta analyse suivant modèle de mcintosh
</commit_message>
<xml_diff>
--- a/meta-analysis-ssa.xlsx
+++ b/meta-analysis-ssa.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28560" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28560" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="56">
   <si>
     <t>Source</t>
   </si>
@@ -128,7 +129,70 @@
     <t>R</t>
   </si>
   <si>
-    <t>2 (early post-test)</t>
+    <t>Sarri (2008)</t>
+  </si>
+  <si>
+    <t>5-10</t>
+  </si>
+  <si>
+    <t>Hatada (2006)</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>STUDY</t>
+  </si>
+  <si>
+    <t>XPT</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>raw_cm</t>
+  </si>
+  <si>
+    <t>raw_deg</t>
+  </si>
+  <si>
+    <t>raw_d</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>prism</t>
+  </si>
+  <si>
+    <t>movement</t>
+  </si>
+  <si>
+    <t>Berberovic2003</t>
+  </si>
+  <si>
+    <t>Striemer2010</t>
+  </si>
+  <si>
+    <t>Herlihey2010</t>
+  </si>
+  <si>
+    <t>Fortis2011</t>
+  </si>
+  <si>
+    <t>Guinet2013</t>
+  </si>
+  <si>
+    <t>Striemer2016</t>
+  </si>
+  <si>
+    <t>Schintu2017</t>
+  </si>
+  <si>
+    <t>Sarri2008</t>
+  </si>
+  <si>
+    <t>Hatada2006</t>
   </si>
 </sst>
 </file>
@@ -160,7 +224,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -177,11 +241,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -190,6 +269,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,31 +576,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.42578125" customWidth="1"/>
     <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.42578125" customWidth="1"/>
     <col min="10" max="10" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.5703125" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" customWidth="1"/>
+    <col min="11" max="12" width="27.5703125" customWidth="1"/>
+    <col min="15" max="16" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="7"/>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
       <c r="E1" s="3" t="s">
@@ -510,19 +616,21 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="3" t="s">
+      <c r="N1" s="3"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
@@ -540,46 +648,50 @@
       <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" t="s">
+      <c r="K2" s="6"/>
+      <c r="L2" s="1"/>
+      <c r="M2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" t="s">
+      <c r="R2" s="6"/>
+      <c r="S2" t="s">
         <v>11</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="J3" t="s">
         <v>16</v>
       </c>
       <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="O3" t="s">
+      <c r="L3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" t="s">
         <v>16</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C4">
@@ -605,17 +717,17 @@
         <f>3.74-0.04</f>
         <v>3.7</v>
       </c>
-      <c r="L4">
-        <f>M4/SQRT(C4)</f>
+      <c r="M4">
+        <f>N4/SQRT(C4)</f>
         <v>1.3673514544549255</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <f>SQRT(((3.62^2)+(4.1^2)))</f>
         <v>5.4694058178197018</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C5">
@@ -641,20 +753,20 @@
         <f>ABS(-1.27 - 2.13)</f>
         <v>3.4</v>
       </c>
-      <c r="L5">
-        <f>M5/SQRT(C5)</f>
+      <c r="M5">
+        <f>N5/SQRT(C5)</f>
         <v>1.4668468307904545</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <f>SQRT(((4.425^2)+(3.853^2)))</f>
         <v>5.8673873231618181</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="8">
         <v>1</v>
       </c>
       <c r="C6">
@@ -676,20 +788,20 @@
         <f>10.3-3.4</f>
         <v>6.9</v>
       </c>
-      <c r="L6">
-        <f>M6/SQRT(C6)</f>
+      <c r="M6">
+        <f>N6/SQRT(C6)</f>
         <v>1.7492855684535902</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <f>SQRT((((1.5*SQRT(8))^2)+((0.9*SQRT(8))^2)))</f>
         <v>4.9477267507411931</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C7">
@@ -710,31 +822,31 @@
       <c r="K7">
         <v>1.6</v>
       </c>
-      <c r="L7">
-        <f>M7/SQRT(C7)</f>
+      <c r="M7">
+        <f>N7/SQRT(C7)</f>
         <v>0.7</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <f>0.7*SQRT(C7)</f>
         <v>3.1304951684997055</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>-1.4</v>
       </c>
-      <c r="Q7">
-        <f>R7/SQRT(C7)</f>
+      <c r="S7">
+        <f>T7/SQRT(C7)</f>
         <v>0.4</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <f>0.4*SQRT(C7)</f>
         <v>1.7888543819998319</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="8">
         <v>1</v>
       </c>
       <c r="C8">
@@ -755,17 +867,17 @@
       <c r="K8">
         <v>1.5</v>
       </c>
-      <c r="L8">
-        <f t="shared" ref="L8:L9" si="0">M8/SQRT(C8)</f>
+      <c r="M8">
+        <f t="shared" ref="M8:M9" si="0">N8/SQRT(C8)</f>
         <v>0.81215762016987814</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <f>SQRT((((0.5*SQRT(28))^2)+((0.64*SQRT(28))^2)))</f>
         <v>4.2975341767111059</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B9">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
         <v>1</v>
       </c>
       <c r="C9">
@@ -786,20 +898,20 @@
       <c r="K9">
         <v>1.81</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f t="shared" si="0"/>
         <v>0.97652444925869619</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <f>SQRT((((0.56*SQRT(28))^2)+((0.8*SQRT(28))^2)))</f>
         <v>5.1672816838256459</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C10">
@@ -820,29 +932,29 @@
       <c r="K10">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L10">
-        <f>M10/SQRT(C10)</f>
+      <c r="M10">
+        <f>N10/SQRT(C10)</f>
         <v>0.22999999999999998</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>0.69</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>-2.87</v>
       </c>
-      <c r="Q10">
-        <f>R10/SQRT(C10)</f>
+      <c r="S10">
+        <f>T10/SQRT(C10)</f>
         <v>0.36000000000000004</v>
       </c>
-      <c r="R10">
+      <c r="T10">
         <v>1.08</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="8">
         <v>1</v>
       </c>
       <c r="C11">
@@ -868,17 +980,17 @@
         <f>(RADIANS(J11))*55</f>
         <v>2.399827721492203</v>
       </c>
-      <c r="L11">
-        <f>M11/SQRT(C11)</f>
+      <c r="M11">
+        <f>N11/SQRT(C11)</f>
         <v>0.93509357820487693</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <f>SQRT((((0.7*SQRT(22))^2)+((0.62*SQRT(22))^2)))</f>
         <v>4.3859776561218373</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B12">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="8">
         <v>1</v>
       </c>
       <c r="C12">
@@ -904,20 +1016,20 @@
         <f>(RADIANS(J12))*55</f>
         <v>5.0492375260195947</v>
       </c>
-      <c r="L12">
-        <f>M12/SQRT(C12)</f>
+      <c r="M12">
+        <f>N12/SQRT(C12)</f>
         <v>1.1540038994734809</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <f>SQRT((((0.925*SQRT(25))^2)+((0.69*SQRT(25))^2)))</f>
         <v>5.7700194973674046</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C13">
@@ -938,18 +1050,18 @@
       <c r="K13">
         <v>4.9000000000000004</v>
       </c>
-      <c r="L13">
-        <f>M13/SQRT(C13)</f>
+      <c r="M13">
+        <f>N13/SQRT(C13)</f>
         <v>0.58600341295934444</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <f>SQRT((((0.53*SQRT(40))^2)+((0.25*SQRT(40))^2)))</f>
         <v>3.7062110031675211</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>34</v>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="C14">
         <v>40</v>
@@ -969,40 +1081,723 @@
       <c r="K14">
         <v>3.8</v>
       </c>
-      <c r="L14">
-        <f>M14/SQRT(C14)</f>
+      <c r="M14">
+        <f>N14/SQRT(C14)</f>
         <v>0.55901699437494745</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <f>SQRT((((0.25*SQRT(40))^2)+((0.5*SQRT(40))^2)))</f>
         <v>3.5355339059327378</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15">
+        <v>80</v>
+      </c>
       <c r="K15">
+        <f>ABS(-5.45--2.14)</f>
+        <v>3.31</v>
+      </c>
+      <c r="M15">
+        <f>N15/SQRT(C15)</f>
+        <v>1.1661903789690602</v>
+      </c>
+      <c r="N15">
+        <f>SQRT((((0.6*SQRT(13))^2)+((1*SQRT(13))^2)))</f>
+        <v>4.2047592083257275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16">
+        <v>320</v>
+      </c>
+      <c r="K16">
+        <f>4.96</f>
+        <v>4.96</v>
+      </c>
+      <c r="M16">
+        <f>N16/SQRT(C16)</f>
+        <v>1.26</v>
+      </c>
+      <c r="N16">
+        <f>1.26*SQRT(7)</f>
+        <v>3.3336466519413843</v>
+      </c>
+      <c r="R16">
+        <v>-4.51</v>
+      </c>
+      <c r="S16">
+        <f>T16/SQRT(C16)</f>
+        <v>0.71</v>
+      </c>
+      <c r="T16">
+        <f>0.71*SQRT(7)</f>
+        <v>1.8784834308558593</v>
+      </c>
+    </row>
+    <row r="17" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K17">
         <f>AVERAGE(K4:K14)</f>
         <v>3.3871877497737994</v>
       </c>
-      <c r="L15">
-        <f t="shared" ref="L15:M15" si="1">AVERAGE(L4:L13)</f>
+      <c r="M17">
+        <f t="shared" ref="M17:N17" si="1">AVERAGE(M4:M13)</f>
         <v>0.99772668137652454</v>
       </c>
-      <c r="M15">
+      <c r="N17">
         <f t="shared" si="1"/>
         <v>4.3432039077415938</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="L16" t="s">
+    <row r="18" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="O25" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="12">
+        <v>16</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="12">
+        <v>10</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="12">
+        <v>200</v>
+      </c>
+      <c r="H2" s="14">
+        <f>3.88 - 0.43</f>
+        <v>3.4499999999999997</v>
+      </c>
+      <c r="I2" s="14">
+        <f>3.74-0.04</f>
+        <v>3.7</v>
+      </c>
+      <c r="J2" s="14">
+        <f>I2/L2</f>
+        <v>0.67649030319621639</v>
+      </c>
+      <c r="K2" s="14">
+        <f>L2/SQRT(C2)</f>
+        <v>1.3673514544549255</v>
+      </c>
+      <c r="L2" s="14">
+        <f>SQRT(((3.62^2)+(4.1^2)))</f>
+        <v>5.4694058178197018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="12">
+        <v>16</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="12">
+        <v>10</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="12">
+        <v>200</v>
+      </c>
+      <c r="H3" s="14">
+        <f>ABS(-1.315-2.203)</f>
+        <v>3.5179999999999998</v>
+      </c>
+      <c r="I3" s="14">
+        <f>ABS(-1.27 - 2.13)</f>
+        <v>3.4</v>
+      </c>
+      <c r="J3" s="14">
+        <f t="shared" ref="J3:J14" si="0">I3/L3</f>
+        <v>0.57947427240371918</v>
+      </c>
+      <c r="K3" s="14">
+        <f>L3/SQRT(C3)</f>
+        <v>1.4668468307904545</v>
+      </c>
+      <c r="L3" s="14">
+        <f>SQRT(((4.425^2)+(3.853^2)))</f>
+        <v>5.8673873231618181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12">
+        <v>8</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="12">
+        <v>10</v>
+      </c>
+      <c r="F4" s="12">
+        <v>10</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14">
+        <f>10.3-3.4</f>
+        <v>6.9</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" si="0"/>
+        <v>1.3945798439589145</v>
+      </c>
+      <c r="K4" s="14">
+        <f>L4/SQRT(C4)</f>
+        <v>1.7492855684535902</v>
+      </c>
+      <c r="L4" s="14">
+        <f>SQRT((((1.5*SQRT(8))^2)+((0.9*SQRT(8))^2)))</f>
+        <v>4.9477267507411931</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="12">
+        <v>20</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="12">
+        <v>10</v>
+      </c>
+      <c r="F5" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="G5" s="12">
+        <v>204</v>
+      </c>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14">
+        <v>1.6</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" si="0"/>
+        <v>0.51110125199995193</v>
+      </c>
+      <c r="K5" s="14">
+        <f>L5/SQRT(C5)</f>
+        <v>0.7</v>
+      </c>
+      <c r="L5" s="14">
+        <f>0.7*SQRT(C5)</f>
+        <v>3.1304951684997055</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="12">
+        <v>1</v>
+      </c>
+      <c r="C6" s="12">
+        <v>28</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="12">
+        <v>12.4</v>
+      </c>
+      <c r="F6" s="12">
+        <v>10</v>
+      </c>
+      <c r="G6" s="12">
+        <v>60</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.34903736382800493</v>
+      </c>
+      <c r="K6" s="14">
+        <f>L6/SQRT(C6)</f>
+        <v>0.81215762016987814</v>
+      </c>
+      <c r="L6" s="14">
+        <f>SQRT((((0.5*SQRT(28))^2)+((0.64*SQRT(28))^2)))</f>
+        <v>4.2975341767111059</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="12">
+        <v>1</v>
+      </c>
+      <c r="C7" s="12">
+        <v>28</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="12">
+        <v>12.4</v>
+      </c>
+      <c r="F7" s="12">
+        <v>10</v>
+      </c>
+      <c r="G7" s="12">
+        <v>60</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14">
+        <v>1.81</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="0"/>
+        <v>0.3502808847571765</v>
+      </c>
+      <c r="K7" s="14">
+        <f>L7/SQRT(C7)</f>
+        <v>0.97652444925869619</v>
+      </c>
+      <c r="L7" s="14">
+        <f>SQRT((((0.56*SQRT(28))^2)+((0.8*SQRT(28))^2)))</f>
+        <v>5.1672816838256459</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="12">
+        <v>9</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="12">
+        <v>15</v>
+      </c>
+      <c r="F8" s="12">
+        <v>15</v>
+      </c>
+      <c r="G8" s="12">
+        <v>540</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J8" s="14">
+        <f t="shared" si="0"/>
+        <v>3.1884057971014497</v>
+      </c>
+      <c r="K8" s="14">
+        <f>L8/SQRT(C8)</f>
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="L8" s="14">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="12">
+        <v>1</v>
+      </c>
+      <c r="C9" s="12">
+        <v>22</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="12">
+        <v>8.5</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="12">
+        <v>200</v>
+      </c>
+      <c r="H9" s="14">
+        <f>4.7-2.2</f>
+        <v>2.5</v>
+      </c>
+      <c r="I9" s="14">
+        <f>(RADIANS(H9))*55</f>
+        <v>2.399827721492203</v>
+      </c>
+      <c r="J9" s="14">
+        <f t="shared" si="0"/>
+        <v>0.54715913067696176</v>
+      </c>
+      <c r="K9" s="14">
+        <f>L9/SQRT(C9)</f>
+        <v>0.93509357820487693</v>
+      </c>
+      <c r="L9" s="14">
+        <f>SQRT((((0.7*SQRT(22))^2)+((0.62*SQRT(22))^2)))</f>
+        <v>4.3859776561218373</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1</v>
+      </c>
+      <c r="C10" s="12">
+        <v>25</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="12">
+        <v>17</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="12">
+        <v>200</v>
+      </c>
+      <c r="H10" s="14">
+        <f>7.93-2.67</f>
+        <v>5.26</v>
+      </c>
+      <c r="I10" s="14">
+        <f>(RADIANS(H10))*55</f>
+        <v>5.0492375260195947</v>
+      </c>
+      <c r="J10" s="14">
+        <f t="shared" si="0"/>
+        <v>0.87508153626228302</v>
+      </c>
+      <c r="K10" s="14">
+        <f>L10/SQRT(C10)</f>
+        <v>1.1540038994734809</v>
+      </c>
+      <c r="L10" s="14">
+        <f>SQRT((((0.925*SQRT(25))^2)+((0.69*SQRT(25))^2)))</f>
+        <v>5.7700194973674046</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="12">
+        <v>40</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="12">
+        <v>15</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="12">
+        <v>150</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J11" s="14">
+        <f t="shared" si="0"/>
+        <v>1.3221049734654085</v>
+      </c>
+      <c r="K11" s="14">
+        <f>L11/SQRT(C11)</f>
+        <v>0.58600341295934444</v>
+      </c>
+      <c r="L11" s="14">
+        <f>SQRT((((0.53*SQRT(40))^2)+((0.25*SQRT(40))^2)))</f>
+        <v>3.7062110031675211</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="12">
+        <v>40</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="12">
+        <v>15</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="12">
+        <v>150</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14">
+        <v>3.8</v>
+      </c>
+      <c r="J12" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0748023074035522</v>
+      </c>
+      <c r="K12" s="14">
+        <f>L12/SQRT(C12)</f>
+        <v>0.55901699437494745</v>
+      </c>
+      <c r="L12" s="14">
+        <f>SQRT((((0.25*SQRT(40))^2)+((0.5*SQRT(40))^2)))</f>
+        <v>3.5355339059327378</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="12">
+        <v>1</v>
+      </c>
+      <c r="C13" s="12">
+        <v>13</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="12">
+        <v>10</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="12">
+        <v>80</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14">
+        <f>ABS(-5.45--2.14)</f>
+        <v>3.31</v>
+      </c>
+      <c r="J13" s="14">
+        <f t="shared" si="0"/>
+        <v>0.78720322282568778</v>
+      </c>
+      <c r="K13" s="14">
+        <f>L13/SQRT(C13)</f>
+        <v>1.1661903789690602</v>
+      </c>
+      <c r="L13" s="14">
+        <f>SQRT((((0.6*SQRT(13))^2)+((1*SQRT(13))^2)))</f>
+        <v>4.2047592083257275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="12">
+        <v>7</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="12">
+        <v>15</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="12">
+        <v>320</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14">
+        <f>4.96</f>
+        <v>4.96</v>
+      </c>
+      <c r="J14" s="14">
+        <f t="shared" si="0"/>
+        <v>1.4878601477188627</v>
+      </c>
+      <c r="K14" s="14">
+        <f>L14/SQRT(C14)</f>
+        <v>1.26</v>
+      </c>
+      <c r="L14" s="14">
+        <f>1.26*SQRT(7)</f>
+        <v>3.3336466519413843</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>